<commit_message>
Format the Course Card
</commit_message>
<xml_diff>
--- a/public/CourseData/Baking.xlsx
+++ b/public/CourseData/Baking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jere\Desktop\ParentGoWhere\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AF46E12-9CF7-4484-AB49-48A7EED0E222}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{534BE530-0A01-41DA-9CCC-82348DEF98EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34400" windowHeight="10530" xr2:uid="{CDB8082C-981C-4481-8C2B-1F4347455684}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7550" xr2:uid="{CDB8082C-981C-4481-8C2B-1F4347455684}"/>
   </bookViews>
   <sheets>
     <sheet name="Baking" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="875">
   <si>
     <t>Course Title</t>
   </si>
@@ -2596,6 +2596,60 @@
   </si>
   <si>
     <t>www.singaporetech.edu.sg</t>
+  </si>
+  <si>
+    <t>/content/dam/portal/tex/aot/hero/21_7.jpg</t>
+  </si>
+  <si>
+    <t>/content/dam/portal/tex/aot/hero/21_2.jpg</t>
+  </si>
+  <si>
+    <t>/content/dam/portal/tex/aot/hero/21_6.jpg</t>
+  </si>
+  <si>
+    <t>/content/dam/portal/tex/aot/hero/1_2.jpg</t>
+  </si>
+  <si>
+    <t>/content/dam/portal/tex/aot/hero/21_8.jpg</t>
+  </si>
+  <si>
+    <t>/content/dam/portal/tex/aot/hero/21_1.jpg</t>
+  </si>
+  <si>
+    <t>/content/dam/portal/tex/aot/hero/21_4.jpg</t>
+  </si>
+  <si>
+    <t>/content/dam/portal/tex/aot/hero/21_10.jpg</t>
+  </si>
+  <si>
+    <t>/content/dam/portal/tex/aot/hero/21_11.jpg</t>
+  </si>
+  <si>
+    <t>/content/dam/portal/tex/aot/hero/21_5.jpg</t>
+  </si>
+  <si>
+    <t>/content/dam/portal/tex/aot/hero/21_9.jpg</t>
+  </si>
+  <si>
+    <t>/content/dam/portal/tex/aot/hero/21_3.jpg</t>
+  </si>
+  <si>
+    <t>/content/dam/portal/tex/aot/hero/999_5.jpg</t>
+  </si>
+  <si>
+    <t>/content/dam/portal/tex/aot/hero/999_3.jpg</t>
+  </si>
+  <si>
+    <t>/content/dam/portal/tex/aot/hero/10_5.jpg</t>
+  </si>
+  <si>
+    <t>/content/dam/portal/tex/aot/hero/999_4.jpg</t>
+  </si>
+  <si>
+    <t>/content/dam/portal/tex/aot/hero/10_3.jpg</t>
+  </si>
+  <si>
+    <t>Image</t>
   </si>
 </sst>
 </file>
@@ -2672,17 +2726,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF333333"/>
+      <left style="thin">
+        <color auto="1"/>
       </left>
-      <right style="medium">
-        <color rgb="FF333333"/>
+      <right style="thin">
+        <color auto="1"/>
       </right>
-      <top style="medium">
-        <color rgb="FF333333"/>
+      <top style="thin">
+        <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF333333"/>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2691,13 +2745,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2705,7 +2759,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -3023,52 +3080,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F18C9F4-D011-49FD-8371-6086AD20D7ED}">
-  <dimension ref="A1:J265"/>
+  <dimension ref="A1:I265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="D147" workbookViewId="0">
+      <selection activeCell="E150" sqref="E150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.1796875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="64.26953125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="37.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" style="2"/>
-    <col min="7" max="7" width="6.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.453125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="36.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="64.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" style="1"/>
+    <col min="7" max="7" width="6.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="35.08984375" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I1" s="2" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -3093,9 +3154,11 @@
       <c r="H2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="5"/>
-    </row>
-    <row r="3" spans="1:10" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I2" s="6" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -3120,8 +3183,11 @@
       <c r="H3" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I3" s="5" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -3146,8 +3212,11 @@
       <c r="H4" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I4" s="5" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
@@ -3172,8 +3241,11 @@
       <c r="H5" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I5" s="5" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
@@ -3198,8 +3270,11 @@
       <c r="H6" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I6" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>31</v>
       </c>
@@ -3224,8 +3299,11 @@
       <c r="H7" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I7" s="5" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>35</v>
       </c>
@@ -3250,8 +3328,11 @@
       <c r="H8" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I8" s="5" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>39</v>
       </c>
@@ -3276,8 +3357,11 @@
       <c r="H9" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I9" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="91" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>42</v>
       </c>
@@ -3302,8 +3386,11 @@
       <c r="H10" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I10" s="5" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="91" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>46</v>
       </c>
@@ -3328,8 +3415,11 @@
       <c r="H11" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I11" s="5" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="78" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>50</v>
       </c>
@@ -3354,8 +3444,11 @@
       <c r="H12" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I12" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>53</v>
       </c>
@@ -3380,8 +3473,11 @@
       <c r="H13" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I13" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>56</v>
       </c>
@@ -3406,8 +3502,11 @@
       <c r="H14" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I14" s="5" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>59</v>
       </c>
@@ -3432,8 +3531,11 @@
       <c r="H15" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I15" s="5" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>63</v>
       </c>
@@ -3458,8 +3560,11 @@
       <c r="H16" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I16" s="5" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>67</v>
       </c>
@@ -3484,8 +3589,11 @@
       <c r="H17" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I17" s="5" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>71</v>
       </c>
@@ -3510,8 +3618,11 @@
       <c r="H18" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I18" s="5" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>74</v>
       </c>
@@ -3536,8 +3647,11 @@
       <c r="H19" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I19" s="5" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>78</v>
       </c>
@@ -3562,8 +3676,11 @@
       <c r="H20" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I20" s="5" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>82</v>
       </c>
@@ -3588,8 +3705,11 @@
       <c r="H21" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I21" s="5" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="78" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>85</v>
       </c>
@@ -3614,8 +3734,11 @@
       <c r="H22" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I22" s="5" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>89</v>
       </c>
@@ -3640,8 +3763,11 @@
       <c r="H23" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I23" s="5" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>92</v>
       </c>
@@ -3666,8 +3792,11 @@
       <c r="H24" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="104.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I24" s="5" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="104" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>96</v>
       </c>
@@ -3692,8 +3821,11 @@
       <c r="H25" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I25" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>100</v>
       </c>
@@ -3718,8 +3850,11 @@
       <c r="H26" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I26" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>103</v>
       </c>
@@ -3744,8 +3879,11 @@
       <c r="H27" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I27" s="5" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>107</v>
       </c>
@@ -3770,8 +3908,11 @@
       <c r="H28" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I28" s="5" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>111</v>
       </c>
@@ -3796,8 +3937,11 @@
       <c r="H29" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I29" s="5" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>114</v>
       </c>
@@ -3822,8 +3966,11 @@
       <c r="H30" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I30" s="5" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>118</v>
       </c>
@@ -3848,8 +3995,11 @@
       <c r="H31" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I31" s="5" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>122</v>
       </c>
@@ -3874,8 +4024,11 @@
       <c r="H32" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I32" s="5" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>126</v>
       </c>
@@ -3900,8 +4053,11 @@
       <c r="H33" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I33" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>130</v>
       </c>
@@ -3926,8 +4082,11 @@
       <c r="H34" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I34" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>133</v>
       </c>
@@ -3952,8 +4111,11 @@
       <c r="H35" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I35" s="5" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>137</v>
       </c>
@@ -3978,8 +4140,11 @@
       <c r="H36" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I36" s="5" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>140</v>
       </c>
@@ -4004,8 +4169,11 @@
       <c r="H37" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I37" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>143</v>
       </c>
@@ -4030,8 +4198,11 @@
       <c r="H38" s="4" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I38" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>149</v>
       </c>
@@ -4056,8 +4227,11 @@
       <c r="H39" s="4" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I39" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="78" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>152</v>
       </c>
@@ -4082,8 +4256,11 @@
       <c r="H40" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" ht="208.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I40" s="5" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="208" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>157</v>
       </c>
@@ -4108,8 +4285,11 @@
       <c r="H41" s="4" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="156.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I41" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="156" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>163</v>
       </c>
@@ -4134,8 +4314,11 @@
       <c r="H42" s="4" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" ht="195.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I42" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="195" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>166</v>
       </c>
@@ -4160,8 +4343,11 @@
       <c r="H43" s="4" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" ht="117.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I43" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="117" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>169</v>
       </c>
@@ -4186,8 +4372,11 @@
       <c r="H44" s="4" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" ht="130.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I44" s="5" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="130" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>172</v>
       </c>
@@ -4212,8 +4401,11 @@
       <c r="H45" s="4" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" ht="104.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I45" s="5" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="104" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>175</v>
       </c>
@@ -4238,8 +4430,11 @@
       <c r="H46" s="4" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I46" s="5" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>178</v>
       </c>
@@ -4264,8 +4459,11 @@
       <c r="H47" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" ht="169.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I47" s="5" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="169" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>183</v>
       </c>
@@ -4290,8 +4488,11 @@
       <c r="H48" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" ht="182.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I48" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="182" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>188</v>
       </c>
@@ -4316,8 +4517,11 @@
       <c r="H49" s="4" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I49" s="5" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>194</v>
       </c>
@@ -4342,8 +4546,11 @@
       <c r="H50" s="4" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I50" s="5" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="104" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>198</v>
       </c>
@@ -4368,8 +4575,11 @@
       <c r="H51" s="4" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I51" s="5" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>202</v>
       </c>
@@ -4394,8 +4604,11 @@
       <c r="H52" s="4" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I52" s="5" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="104" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>205</v>
       </c>
@@ -4420,8 +4633,11 @@
       <c r="H53" s="4" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" ht="182.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I53" s="5" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="182" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>207</v>
       </c>
@@ -4446,8 +4662,11 @@
       <c r="H54" s="4" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I54" s="5" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>210</v>
       </c>
@@ -4472,8 +4691,11 @@
       <c r="H55" s="4" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I55" s="5" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
         <v>214</v>
       </c>
@@ -4498,8 +4720,11 @@
       <c r="H56" s="4" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I56" s="5" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
         <v>218</v>
       </c>
@@ -4524,8 +4749,11 @@
       <c r="H57" s="4" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" ht="195.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I57" s="5" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="195" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
         <v>221</v>
       </c>
@@ -4550,8 +4778,11 @@
       <c r="H58" s="4" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" ht="130.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I58" s="5" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="130" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
         <v>225</v>
       </c>
@@ -4576,8 +4807,11 @@
       <c r="H59" s="4" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I59" s="5" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="91" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
         <v>229</v>
       </c>
@@ -4602,8 +4836,11 @@
       <c r="H60" s="4" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" ht="130.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I60" s="5" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="130" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>232</v>
       </c>
@@ -4628,8 +4865,11 @@
       <c r="H61" s="4" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I61" s="5" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="91" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
         <v>234</v>
       </c>
@@ -4654,8 +4894,11 @@
       <c r="H62" s="4" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" ht="169.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I62" s="5" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="169" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
         <v>183</v>
       </c>
@@ -4680,8 +4923,11 @@
       <c r="H63" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I63" s="5" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
         <v>239</v>
       </c>
@@ -4706,8 +4952,11 @@
       <c r="H64" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I64" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>178</v>
       </c>
@@ -4732,8 +4981,11 @@
       <c r="H65" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" ht="169.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I65" s="5" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="169" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
         <v>183</v>
       </c>
@@ -4758,8 +5010,11 @@
       <c r="H66" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I66" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
         <v>178</v>
       </c>
@@ -4784,8 +5039,11 @@
       <c r="H67" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" ht="169.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I67" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="169" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
         <v>183</v>
       </c>
@@ -4810,8 +5068,11 @@
       <c r="H68" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I68" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
         <v>178</v>
       </c>
@@ -4836,8 +5097,11 @@
       <c r="H69" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I69" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
         <v>252</v>
       </c>
@@ -4862,8 +5126,11 @@
       <c r="H70" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I70" s="5" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
         <v>255</v>
       </c>
@@ -4888,8 +5155,11 @@
       <c r="H71" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I71" s="5" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
         <v>259</v>
       </c>
@@ -4914,8 +5184,11 @@
       <c r="H72" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I72" s="5" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
         <v>262</v>
       </c>
@@ -4940,8 +5213,11 @@
       <c r="H73" s="4" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I73" s="5" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
         <v>268</v>
       </c>
@@ -4966,8 +5242,11 @@
       <c r="H74" s="4" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I74" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>271</v>
       </c>
@@ -4992,8 +5271,11 @@
       <c r="H75" s="4" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" ht="182.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I75" s="5" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="182" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
         <v>274</v>
       </c>
@@ -5018,8 +5300,11 @@
       <c r="H76" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I76" s="5" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="s">
         <v>255</v>
       </c>
@@ -5044,8 +5329,11 @@
       <c r="H77" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I77" s="5" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
         <v>178</v>
       </c>
@@ -5070,8 +5358,11 @@
       <c r="H78" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I78" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
         <v>239</v>
       </c>
@@ -5096,8 +5387,11 @@
       <c r="H79" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" ht="169.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I79" s="5" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="169" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
         <v>183</v>
       </c>
@@ -5122,8 +5416,11 @@
       <c r="H80" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I80" s="5" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
         <v>178</v>
       </c>
@@ -5148,8 +5445,11 @@
       <c r="H81" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I81" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
         <v>252</v>
       </c>
@@ -5174,8 +5474,11 @@
       <c r="H82" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I82" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
         <v>255</v>
       </c>
@@ -5200,8 +5503,11 @@
       <c r="H83" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I83" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
         <v>178</v>
       </c>
@@ -5226,8 +5532,11 @@
       <c r="H84" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I84" s="5" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
         <v>289</v>
       </c>
@@ -5252,8 +5561,11 @@
       <c r="H85" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I85" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
         <v>295</v>
       </c>
@@ -5278,8 +5590,11 @@
       <c r="H86" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I86" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
         <v>298</v>
       </c>
@@ -5304,8 +5619,11 @@
       <c r="H87" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I87" s="5" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
         <v>301</v>
       </c>
@@ -5330,8 +5648,11 @@
       <c r="H88" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I88" s="5" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="78" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
         <v>304</v>
       </c>
@@ -5356,8 +5677,11 @@
       <c r="H89" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I89" s="5" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
         <v>307</v>
       </c>
@@ -5382,8 +5706,11 @@
       <c r="H90" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I90" s="5" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
         <v>310</v>
       </c>
@@ -5408,8 +5735,11 @@
       <c r="H91" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I91" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
         <v>314</v>
       </c>
@@ -5434,8 +5764,11 @@
       <c r="H92" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I92" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
         <v>317</v>
       </c>
@@ -5460,8 +5793,11 @@
       <c r="H93" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I93" s="5" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
         <v>320</v>
       </c>
@@ -5486,8 +5822,11 @@
       <c r="H94" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I94" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
         <v>323</v>
       </c>
@@ -5512,8 +5851,11 @@
       <c r="H95" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I95" s="5" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
         <v>326</v>
       </c>
@@ -5538,8 +5880,11 @@
       <c r="H96" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I96" s="5" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="s">
         <v>329</v>
       </c>
@@ -5564,8 +5909,11 @@
       <c r="H97" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I97" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
         <v>332</v>
       </c>
@@ -5590,8 +5938,11 @@
       <c r="H98" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I98" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
         <v>335</v>
       </c>
@@ -5616,8 +5967,11 @@
       <c r="H99" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I99" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="91" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
         <v>338</v>
       </c>
@@ -5642,8 +5996,11 @@
       <c r="H100" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I100" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
         <v>341</v>
       </c>
@@ -5668,8 +6025,11 @@
       <c r="H101" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I101" s="5" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
         <v>344</v>
       </c>
@@ -5694,8 +6054,11 @@
       <c r="H102" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I102" s="5" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
         <v>347</v>
       </c>
@@ -5720,8 +6083,11 @@
       <c r="H103" s="4" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I103" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="s">
         <v>352</v>
       </c>
@@ -5746,8 +6112,11 @@
       <c r="H104" s="4" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I104" s="5" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A105" s="3" t="s">
         <v>355</v>
       </c>
@@ -5772,8 +6141,11 @@
       <c r="H105" s="4" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I105" s="5" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A106" s="3" t="s">
         <v>360</v>
       </c>
@@ -5798,8 +6170,11 @@
       <c r="H106" s="4" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" ht="104.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I106" s="5" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="104" x14ac:dyDescent="0.35">
       <c r="A107" s="3" t="s">
         <v>56</v>
       </c>
@@ -5824,8 +6199,11 @@
       <c r="H107" s="4" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I107" s="5" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A108" s="3" t="s">
         <v>367</v>
       </c>
@@ -5850,8 +6228,11 @@
       <c r="H108" s="4" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I108" s="5" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="s">
         <v>370</v>
       </c>
@@ -5876,8 +6257,11 @@
       <c r="H109" s="4" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" ht="104.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I109" s="5" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="104" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="s">
         <v>373</v>
       </c>
@@ -5902,8 +6286,11 @@
       <c r="H110" s="4" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I110" s="5" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" ht="91" x14ac:dyDescent="0.35">
       <c r="A111" s="3" t="s">
         <v>376</v>
       </c>
@@ -5928,8 +6315,11 @@
       <c r="H111" s="4" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I111" s="5" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A112" s="3" t="s">
         <v>379</v>
       </c>
@@ -5954,8 +6344,11 @@
       <c r="H112" s="4" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" ht="143.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I112" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="143" x14ac:dyDescent="0.35">
       <c r="A113" s="3" t="s">
         <v>382</v>
       </c>
@@ -5980,8 +6373,11 @@
       <c r="H113" s="4" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I113" s="5" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" ht="78" x14ac:dyDescent="0.35">
       <c r="A114" s="3" t="s">
         <v>385</v>
       </c>
@@ -6006,8 +6402,11 @@
       <c r="H114" s="4" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" ht="156.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I114" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" ht="156" x14ac:dyDescent="0.35">
       <c r="A115" s="3" t="s">
         <v>391</v>
       </c>
@@ -6032,8 +6431,11 @@
       <c r="H115" s="4" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" ht="143.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I115" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" ht="143" x14ac:dyDescent="0.35">
       <c r="A116" s="3" t="s">
         <v>395</v>
       </c>
@@ -6058,8 +6460,11 @@
       <c r="H116" s="4" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" ht="169.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I116" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="169" x14ac:dyDescent="0.35">
       <c r="A117" s="3" t="s">
         <v>398</v>
       </c>
@@ -6084,8 +6489,11 @@
       <c r="H117" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" ht="117.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I117" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" ht="117" x14ac:dyDescent="0.35">
       <c r="A118" s="3" t="s">
         <v>402</v>
       </c>
@@ -6110,8 +6518,11 @@
       <c r="H118" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I118" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A119" s="3" t="s">
         <v>405</v>
       </c>
@@ -6136,8 +6547,11 @@
       <c r="H119" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I119" s="5" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A120" s="3" t="s">
         <v>409</v>
       </c>
@@ -6162,8 +6576,11 @@
       <c r="H120" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="121" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I120" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A121" s="3" t="s">
         <v>412</v>
       </c>
@@ -6188,8 +6605,11 @@
       <c r="H121" s="4" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" ht="169.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I121" s="5" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" ht="169" x14ac:dyDescent="0.35">
       <c r="A122" s="3" t="s">
         <v>78</v>
       </c>
@@ -6214,8 +6634,11 @@
       <c r="H122" s="4" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I122" s="5" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A123" s="3" t="s">
         <v>35</v>
       </c>
@@ -6240,8 +6663,11 @@
       <c r="H123" s="4" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" ht="169.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I123" s="5" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" ht="169" x14ac:dyDescent="0.35">
       <c r="A124" s="3" t="s">
         <v>423</v>
       </c>
@@ -6266,8 +6692,11 @@
       <c r="H124" s="4" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" ht="169.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I124" s="5" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" ht="169" x14ac:dyDescent="0.35">
       <c r="A125" s="3" t="s">
         <v>426</v>
       </c>
@@ -6292,8 +6721,11 @@
       <c r="H125" s="4" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="126" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I125" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A126" s="3" t="s">
         <v>429</v>
       </c>
@@ -6318,8 +6750,11 @@
       <c r="H126" s="4" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" ht="169.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I126" s="5" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" ht="169" x14ac:dyDescent="0.35">
       <c r="A127" s="3" t="s">
         <v>56</v>
       </c>
@@ -6344,8 +6779,11 @@
       <c r="H127" s="4" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="128" spans="1:8" ht="156.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I127" s="5" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" ht="156" x14ac:dyDescent="0.35">
       <c r="A128" s="3" t="s">
         <v>434</v>
       </c>
@@ -6370,8 +6808,11 @@
       <c r="H128" s="4" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" ht="169.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I128" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" ht="169" x14ac:dyDescent="0.35">
       <c r="A129" s="3" t="s">
         <v>438</v>
       </c>
@@ -6396,8 +6837,11 @@
       <c r="H129" s="4" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="130" spans="1:8" ht="117.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I129" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" ht="130" x14ac:dyDescent="0.35">
       <c r="A130" s="3" t="s">
         <v>441</v>
       </c>
@@ -6422,8 +6866,11 @@
       <c r="H130" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="131" spans="1:8" ht="156.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I130" s="5" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" ht="156" x14ac:dyDescent="0.35">
       <c r="A131" s="3" t="s">
         <v>445</v>
       </c>
@@ -6448,8 +6895,11 @@
       <c r="H131" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="132" spans="1:8" ht="117.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I131" s="5" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" ht="117" x14ac:dyDescent="0.35">
       <c r="A132" s="3" t="s">
         <v>448</v>
       </c>
@@ -6474,8 +6924,11 @@
       <c r="H132" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" ht="104.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I132" s="5" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" ht="104" x14ac:dyDescent="0.35">
       <c r="A133" s="3" t="s">
         <v>451</v>
       </c>
@@ -6500,8 +6953,11 @@
       <c r="H133" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="134" spans="1:8" ht="169.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I133" s="5" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" ht="169" x14ac:dyDescent="0.35">
       <c r="A134" s="3" t="s">
         <v>454</v>
       </c>
@@ -6526,8 +6982,11 @@
       <c r="H134" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="135" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I134" s="5" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A135" s="3" t="s">
         <v>457</v>
       </c>
@@ -6552,8 +7011,11 @@
       <c r="H135" s="4" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="136" spans="1:8" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I135" s="5" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" ht="91" x14ac:dyDescent="0.35">
       <c r="A136" s="3" t="s">
         <v>462</v>
       </c>
@@ -6578,8 +7040,11 @@
       <c r="H136" s="4" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="137" spans="1:8" ht="169.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I136" s="5" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" ht="169" x14ac:dyDescent="0.35">
       <c r="A137" s="3" t="s">
         <v>467</v>
       </c>
@@ -6604,8 +7069,11 @@
       <c r="H137" s="4" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="138" spans="1:8" ht="156.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I137" s="5" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" ht="156" x14ac:dyDescent="0.35">
       <c r="A138" s="3" t="s">
         <v>469</v>
       </c>
@@ -6630,8 +7098,11 @@
       <c r="H138" s="4" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="139" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I138" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A139" s="3" t="s">
         <v>472</v>
       </c>
@@ -6656,8 +7127,11 @@
       <c r="H139" s="4" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="140" spans="1:8" ht="130.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I139" s="5" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" ht="130" x14ac:dyDescent="0.35">
       <c r="A140" s="3" t="s">
         <v>475</v>
       </c>
@@ -6682,8 +7156,11 @@
       <c r="H140" s="4" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="141" spans="1:8" ht="117.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I140" s="5" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" ht="117" x14ac:dyDescent="0.35">
       <c r="A141" s="3" t="s">
         <v>478</v>
       </c>
@@ -6708,8 +7185,11 @@
       <c r="H141" s="4" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="142" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I141" s="5" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A142" s="3" t="s">
         <v>481</v>
       </c>
@@ -6734,8 +7214,11 @@
       <c r="H142" s="4" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="143" spans="1:8" ht="169.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I142" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" ht="169" x14ac:dyDescent="0.35">
       <c r="A143" s="3" t="s">
         <v>484</v>
       </c>
@@ -6760,8 +7243,11 @@
       <c r="H143" s="4" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="144" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I143" s="5" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A144" s="3" t="s">
         <v>487</v>
       </c>
@@ -6786,8 +7272,11 @@
       <c r="H144" s="4" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="145" spans="1:8" ht="156.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I144" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" ht="156" x14ac:dyDescent="0.35">
       <c r="A145" s="3" t="s">
         <v>490</v>
       </c>
@@ -6812,8 +7301,11 @@
       <c r="H145" s="4" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="146" spans="1:8" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I145" s="5" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" ht="78" x14ac:dyDescent="0.35">
       <c r="A146" s="3" t="s">
         <v>492</v>
       </c>
@@ -6838,8 +7330,11 @@
       <c r="H146" s="4" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="147" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I146" s="5" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A147" s="3" t="s">
         <v>252</v>
       </c>
@@ -6864,8 +7359,11 @@
       <c r="H147" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="148" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I147" s="5" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A148" s="3" t="s">
         <v>255</v>
       </c>
@@ -6890,8 +7388,11 @@
       <c r="H148" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="149" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I148" s="5" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A149" s="3" t="s">
         <v>178</v>
       </c>
@@ -6916,8 +7417,11 @@
       <c r="H149" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="150" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I149" s="5" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A150" s="3" t="s">
         <v>490</v>
       </c>
@@ -6942,8 +7446,11 @@
       <c r="H150" s="4" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="151" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I150" s="5" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A151" s="3" t="s">
         <v>118</v>
       </c>
@@ -6968,8 +7475,11 @@
       <c r="H151" s="4" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="152" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I151" s="5" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A152" s="3" t="s">
         <v>35</v>
       </c>
@@ -6994,8 +7504,11 @@
       <c r="H152" s="4" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="153" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I152" s="5" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A153" s="3" t="s">
         <v>510</v>
       </c>
@@ -7020,8 +7533,11 @@
       <c r="H153" s="4" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="154" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I153" s="5" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A154" s="3" t="s">
         <v>513</v>
       </c>
@@ -7046,8 +7562,11 @@
       <c r="H154" s="4" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="155" spans="1:8" ht="143.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I154" s="5" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" ht="143" x14ac:dyDescent="0.35">
       <c r="A155" s="3" t="s">
         <v>490</v>
       </c>
@@ -7072,8 +7591,11 @@
       <c r="H155" s="4" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="156" spans="1:8" ht="156.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I155" s="5" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" ht="156" x14ac:dyDescent="0.35">
       <c r="A156" s="3" t="s">
         <v>520</v>
       </c>
@@ -7098,8 +7620,11 @@
       <c r="H156" s="4" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="157" spans="1:8" ht="143.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I156" s="5" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" ht="143" x14ac:dyDescent="0.35">
       <c r="A157" s="3" t="s">
         <v>118</v>
       </c>
@@ -7124,8 +7649,11 @@
       <c r="H157" s="4" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="158" spans="1:8" ht="182.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I157" s="5" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" ht="182" x14ac:dyDescent="0.35">
       <c r="A158" s="3" t="s">
         <v>525</v>
       </c>
@@ -7150,8 +7678,11 @@
       <c r="H158" s="4" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="159" spans="1:8" ht="130.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I158" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" ht="130" x14ac:dyDescent="0.35">
       <c r="A159" s="3" t="s">
         <v>35</v>
       </c>
@@ -7176,8 +7707,11 @@
       <c r="H159" s="4" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="160" spans="1:8" ht="156.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I159" s="5" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" ht="156" x14ac:dyDescent="0.35">
       <c r="A160" s="3" t="s">
         <v>56</v>
       </c>
@@ -7202,8 +7736,11 @@
       <c r="H160" s="4" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="161" spans="1:8" ht="156.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I160" s="5" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" ht="156" x14ac:dyDescent="0.35">
       <c r="A161" s="3" t="s">
         <v>531</v>
       </c>
@@ -7228,8 +7765,11 @@
       <c r="H161" s="4" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="162" spans="1:8" ht="156.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I161" s="5" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" ht="156" x14ac:dyDescent="0.35">
       <c r="A162" s="3" t="s">
         <v>78</v>
       </c>
@@ -7254,8 +7794,11 @@
       <c r="H162" s="4" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="163" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I162" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A163" s="3" t="s">
         <v>536</v>
       </c>
@@ -7280,8 +7823,11 @@
       <c r="H163" s="4" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="164" spans="1:8" ht="156.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I163" s="5" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" ht="156" x14ac:dyDescent="0.35">
       <c r="A164" s="3" t="s">
         <v>539</v>
       </c>
@@ -7306,8 +7852,11 @@
       <c r="H164" s="4" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="165" spans="1:8" ht="169.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I164" s="5" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" ht="169" x14ac:dyDescent="0.35">
       <c r="A165" s="3" t="s">
         <v>183</v>
       </c>
@@ -7332,8 +7881,11 @@
       <c r="H165" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="166" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I165" s="5" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A166" s="3" t="s">
         <v>544</v>
       </c>
@@ -7358,8 +7910,11 @@
       <c r="H166" s="4" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="167" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I166" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A167" s="3" t="s">
         <v>549</v>
       </c>
@@ -7384,8 +7939,11 @@
       <c r="H167" s="4" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="168" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I167" s="5" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A168" s="3" t="s">
         <v>552</v>
       </c>
@@ -7410,8 +7968,11 @@
       <c r="H168" s="4" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="169" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I168" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A169" s="3" t="s">
         <v>555</v>
       </c>
@@ -7436,8 +7997,11 @@
       <c r="H169" s="4" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="170" spans="1:8" ht="130.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I169" s="5" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" ht="130" x14ac:dyDescent="0.35">
       <c r="A170" s="3" t="s">
         <v>560</v>
       </c>
@@ -7462,8 +8026,11 @@
       <c r="H170" s="4" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="171" spans="1:8" ht="104.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I170" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" ht="104" x14ac:dyDescent="0.35">
       <c r="A171" s="3" t="s">
         <v>481</v>
       </c>
@@ -7488,8 +8055,11 @@
       <c r="H171" s="4" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="172" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I171" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A172" s="3" t="s">
         <v>490</v>
       </c>
@@ -7514,8 +8084,11 @@
       <c r="H172" s="4" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="173" spans="1:8" ht="104.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I172" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" ht="104" x14ac:dyDescent="0.35">
       <c r="A173" s="3" t="s">
         <v>567</v>
       </c>
@@ -7540,8 +8113,11 @@
       <c r="H173" s="4" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="174" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I173" s="5" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A174" s="3" t="s">
         <v>467</v>
       </c>
@@ -7566,8 +8142,11 @@
       <c r="H174" s="4" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="175" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I174" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A175" s="3" t="s">
         <v>572</v>
       </c>
@@ -7592,8 +8171,11 @@
       <c r="H175" s="4" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="176" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I175" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A176" s="3" t="s">
         <v>536</v>
       </c>
@@ -7618,8 +8200,11 @@
       <c r="H176" s="4" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="177" spans="1:8" ht="104.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I176" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" ht="104" x14ac:dyDescent="0.35">
       <c r="A177" s="3" t="s">
         <v>56</v>
       </c>
@@ -7644,8 +8229,11 @@
       <c r="H177" s="4" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="178" spans="1:8" ht="143.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I177" s="5" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" ht="143" x14ac:dyDescent="0.35">
       <c r="A178" s="3" t="s">
         <v>539</v>
       </c>
@@ -7670,8 +8258,11 @@
       <c r="H178" s="4" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="179" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I178" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A179" s="3" t="s">
         <v>581</v>
       </c>
@@ -7696,8 +8287,11 @@
       <c r="H179" s="4" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="180" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I179" s="5" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A180" s="3" t="s">
         <v>531</v>
       </c>
@@ -7722,8 +8316,11 @@
       <c r="H180" s="4" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="181" spans="1:8" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I180" s="5" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" ht="91" x14ac:dyDescent="0.35">
       <c r="A181" s="3" t="s">
         <v>586</v>
       </c>
@@ -7748,8 +8345,11 @@
       <c r="H181" s="4" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="182" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I181" s="5" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A182" s="3" t="s">
         <v>589</v>
       </c>
@@ -7774,8 +8374,11 @@
       <c r="H182" s="4" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="183" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I182" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A183" s="3" t="s">
         <v>118</v>
       </c>
@@ -7800,8 +8403,11 @@
       <c r="H183" s="4" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="184" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I183" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A184" s="3" t="s">
         <v>595</v>
       </c>
@@ -7826,8 +8432,11 @@
       <c r="H184" s="4" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="185" spans="1:8" ht="143.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I184" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" ht="143" x14ac:dyDescent="0.35">
       <c r="A185" s="3" t="s">
         <v>598</v>
       </c>
@@ -7852,8 +8461,11 @@
       <c r="H185" s="4" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="186" spans="1:8" ht="169.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I185" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" ht="169" x14ac:dyDescent="0.35">
       <c r="A186" s="3" t="s">
         <v>601</v>
       </c>
@@ -7878,8 +8490,11 @@
       <c r="H186" s="4" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="187" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I186" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A187" s="3" t="s">
         <v>604</v>
       </c>
@@ -7904,8 +8519,11 @@
       <c r="H187" s="4" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="188" spans="1:8" ht="169.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I187" s="5" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" ht="169" x14ac:dyDescent="0.35">
       <c r="A188" s="3" t="s">
         <v>607</v>
       </c>
@@ -7930,8 +8548,11 @@
       <c r="H188" s="4" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="189" spans="1:8" ht="143.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I188" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" ht="143" x14ac:dyDescent="0.35">
       <c r="A189" s="3" t="s">
         <v>610</v>
       </c>
@@ -7956,8 +8577,11 @@
       <c r="H189" s="4" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="190" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I189" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A190" s="3" t="s">
         <v>613</v>
       </c>
@@ -7982,8 +8606,11 @@
       <c r="H190" s="4" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="191" spans="1:8" ht="104.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I190" s="5" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" ht="104" x14ac:dyDescent="0.35">
       <c r="A191" s="3" t="s">
         <v>618</v>
       </c>
@@ -8008,8 +8635,11 @@
       <c r="H191" s="4" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="192" spans="1:8" ht="156.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I191" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" ht="156" x14ac:dyDescent="0.35">
       <c r="A192" s="3" t="s">
         <v>621</v>
       </c>
@@ -8034,8 +8664,11 @@
       <c r="H192" s="4" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="193" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I192" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A193" s="3" t="s">
         <v>624</v>
       </c>
@@ -8060,8 +8693,11 @@
       <c r="H193" s="4" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="194" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I193" s="5" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A194" s="3" t="s">
         <v>627</v>
       </c>
@@ -8086,8 +8722,11 @@
       <c r="H194" s="4" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="195" spans="1:8" ht="117.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I194" s="5" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" ht="117" x14ac:dyDescent="0.35">
       <c r="A195" s="3" t="s">
         <v>630</v>
       </c>
@@ -8112,8 +8751,11 @@
       <c r="H195" s="4" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="196" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I195" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A196" s="3" t="s">
         <v>633</v>
       </c>
@@ -8138,8 +8780,11 @@
       <c r="H196" s="4" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="197" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I196" s="5" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A197" s="3" t="s">
         <v>636</v>
       </c>
@@ -8164,8 +8809,11 @@
       <c r="H197" s="4" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="198" spans="1:8" ht="117.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I197" s="5" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" ht="117" x14ac:dyDescent="0.35">
       <c r="A198" s="3" t="s">
         <v>639</v>
       </c>
@@ -8190,8 +8838,11 @@
       <c r="H198" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="199" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I198" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A199" s="3" t="s">
         <v>643</v>
       </c>
@@ -8216,8 +8867,11 @@
       <c r="H199" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="200" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I199" s="5" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A200" s="3" t="s">
         <v>646</v>
       </c>
@@ -8242,8 +8896,11 @@
       <c r="H200" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="201" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I200" s="5" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A201" s="3" t="s">
         <v>649</v>
       </c>
@@ -8268,8 +8925,11 @@
       <c r="H201" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="202" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I201" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A202" s="3" t="s">
         <v>652</v>
       </c>
@@ -8294,8 +8954,11 @@
       <c r="H202" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="203" spans="1:8" ht="182.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I202" s="5" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" ht="182" x14ac:dyDescent="0.35">
       <c r="A203" s="3" t="s">
         <v>655</v>
       </c>
@@ -8320,8 +8983,11 @@
       <c r="H203" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="204" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I203" s="5" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A204" s="3" t="s">
         <v>658</v>
       </c>
@@ -8346,8 +9012,11 @@
       <c r="H204" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="205" spans="1:8" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I204" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" ht="91" x14ac:dyDescent="0.35">
       <c r="A205" s="3" t="s">
         <v>661</v>
       </c>
@@ -8372,8 +9041,11 @@
       <c r="H205" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="206" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I205" s="5" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A206" s="3" t="s">
         <v>664</v>
       </c>
@@ -8398,8 +9070,11 @@
       <c r="H206" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="207" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I206" s="5" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A207" s="3" t="s">
         <v>667</v>
       </c>
@@ -8424,8 +9099,11 @@
       <c r="H207" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="208" spans="1:8" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I207" s="5" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" ht="78" x14ac:dyDescent="0.35">
       <c r="A208" s="3" t="s">
         <v>539</v>
       </c>
@@ -8450,8 +9128,11 @@
       <c r="H208" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="209" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I208" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A209" s="3" t="s">
         <v>673</v>
       </c>
@@ -8476,8 +9157,11 @@
       <c r="H209" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="210" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I209" s="5" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A210" s="3" t="s">
         <v>678</v>
       </c>
@@ -8502,8 +9186,11 @@
       <c r="H210" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="211" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I210" s="5" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A211" s="3" t="s">
         <v>681</v>
       </c>
@@ -8528,8 +9215,11 @@
       <c r="H211" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="212" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I211" s="5" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A212" s="3" t="s">
         <v>684</v>
       </c>
@@ -8554,8 +9244,11 @@
       <c r="H212" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="213" spans="1:8" ht="156.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I212" s="5" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" ht="156" x14ac:dyDescent="0.35">
       <c r="A213" s="3" t="s">
         <v>687</v>
       </c>
@@ -8580,8 +9273,11 @@
       <c r="H213" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="214" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I213" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A214" s="3" t="s">
         <v>690</v>
       </c>
@@ -8606,8 +9302,11 @@
       <c r="H214" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="215" spans="1:8" ht="143.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I214" s="5" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" ht="143" x14ac:dyDescent="0.35">
       <c r="A215" s="3" t="s">
         <v>693</v>
       </c>
@@ -8632,8 +9331,11 @@
       <c r="H215" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="216" spans="1:8" ht="104.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I215" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" ht="104" x14ac:dyDescent="0.35">
       <c r="A216" s="3" t="s">
         <v>696</v>
       </c>
@@ -8658,8 +9360,11 @@
       <c r="H216" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="217" spans="1:8" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I216" s="5" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" ht="78" x14ac:dyDescent="0.35">
       <c r="A217" s="3" t="s">
         <v>700</v>
       </c>
@@ -8684,8 +9389,11 @@
       <c r="H217" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="218" spans="1:8" ht="143.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I217" s="5" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9" ht="143" x14ac:dyDescent="0.35">
       <c r="A218" s="3" t="s">
         <v>704</v>
       </c>
@@ -8710,8 +9418,11 @@
       <c r="H218" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="219" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I218" s="5" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A219" s="3" t="s">
         <v>198</v>
       </c>
@@ -8736,8 +9447,11 @@
       <c r="H219" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="220" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I219" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A220" s="3" t="s">
         <v>710</v>
       </c>
@@ -8762,8 +9476,11 @@
       <c r="H220" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="221" spans="1:8" ht="117.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I220" s="5" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" ht="117" x14ac:dyDescent="0.35">
       <c r="A221" s="3" t="s">
         <v>713</v>
       </c>
@@ -8788,8 +9505,11 @@
       <c r="H221" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="222" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I221" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A222" s="3" t="s">
         <v>716</v>
       </c>
@@ -8814,8 +9534,11 @@
       <c r="H222" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="223" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I222" s="5" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A223" s="3" t="s">
         <v>719</v>
       </c>
@@ -8840,8 +9563,11 @@
       <c r="H223" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="224" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I223" s="5" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A224" s="3" t="s">
         <v>721</v>
       </c>
@@ -8866,8 +9592,11 @@
       <c r="H224" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="225" spans="1:8" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I224" s="5" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9" ht="78" x14ac:dyDescent="0.35">
       <c r="A225" s="3" t="s">
         <v>725</v>
       </c>
@@ -8892,8 +9621,11 @@
       <c r="H225" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="226" spans="1:8" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I225" s="5" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="226" spans="1:9" ht="91" x14ac:dyDescent="0.35">
       <c r="A226" s="3" t="s">
         <v>728</v>
       </c>
@@ -8918,8 +9650,11 @@
       <c r="H226" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="227" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I226" s="5" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="227" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A227" s="3" t="s">
         <v>731</v>
       </c>
@@ -8944,8 +9679,11 @@
       <c r="H227" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="228" spans="1:8" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I227" s="5" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="228" spans="1:9" ht="78" x14ac:dyDescent="0.35">
       <c r="A228" s="3" t="s">
         <v>734</v>
       </c>
@@ -8970,8 +9708,11 @@
       <c r="H228" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="229" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I228" s="5" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="229" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A229" s="3" t="s">
         <v>737</v>
       </c>
@@ -8996,8 +9737,11 @@
       <c r="H229" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="230" spans="1:8" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I229" s="5" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="230" spans="1:9" ht="91" x14ac:dyDescent="0.35">
       <c r="A230" s="3" t="s">
         <v>740</v>
       </c>
@@ -9022,8 +9766,11 @@
       <c r="H230" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="231" spans="1:8" ht="117.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I230" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="231" spans="1:9" ht="117" x14ac:dyDescent="0.35">
       <c r="A231" s="3" t="s">
         <v>743</v>
       </c>
@@ -9048,8 +9795,11 @@
       <c r="H231" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="232" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I231" s="5" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A232" s="3" t="s">
         <v>746</v>
       </c>
@@ -9074,8 +9824,11 @@
       <c r="H232" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="233" spans="1:8" ht="156.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I232" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="233" spans="1:9" ht="156" x14ac:dyDescent="0.35">
       <c r="A233" s="3" t="s">
         <v>749</v>
       </c>
@@ -9100,8 +9853,11 @@
       <c r="H233" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="234" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I233" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="234" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A234" s="3" t="s">
         <v>752</v>
       </c>
@@ -9126,8 +9882,11 @@
       <c r="H234" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="235" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I234" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="235" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A235" s="3" t="s">
         <v>755</v>
       </c>
@@ -9152,8 +9911,11 @@
       <c r="H235" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="236" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I235" s="5" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A236" s="3" t="s">
         <v>758</v>
       </c>
@@ -9178,8 +9940,11 @@
       <c r="H236" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="237" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I236" s="5" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A237" s="3" t="s">
         <v>760</v>
       </c>
@@ -9204,8 +9969,11 @@
       <c r="H237" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="238" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I237" s="5" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A238" s="3" t="s">
         <v>763</v>
       </c>
@@ -9230,8 +9998,11 @@
       <c r="H238" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="239" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I238" s="5" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A239" s="3" t="s">
         <v>766</v>
       </c>
@@ -9256,8 +10027,11 @@
       <c r="H239" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="240" spans="1:8" ht="104.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I239" s="5" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9" ht="104" x14ac:dyDescent="0.35">
       <c r="A240" s="3" t="s">
         <v>769</v>
       </c>
@@ -9282,8 +10056,11 @@
       <c r="H240" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="241" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I240" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="241" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A241" s="3" t="s">
         <v>773</v>
       </c>
@@ -9308,8 +10085,11 @@
       <c r="H241" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="242" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I241" s="5" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="242" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A242" s="3" t="s">
         <v>776</v>
       </c>
@@ -9334,8 +10114,11 @@
       <c r="H242" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="243" spans="1:8" ht="247.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I242" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="243" spans="1:9" ht="247" x14ac:dyDescent="0.35">
       <c r="A243" s="3" t="s">
         <v>779</v>
       </c>
@@ -9360,8 +10143,11 @@
       <c r="H243" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="244" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I243" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="244" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A244" s="3" t="s">
         <v>783</v>
       </c>
@@ -9386,8 +10172,11 @@
       <c r="H244" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="245" spans="1:8" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I244" s="5" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="245" spans="1:9" ht="91" x14ac:dyDescent="0.35">
       <c r="A245" s="3" t="s">
         <v>539</v>
       </c>
@@ -9412,8 +10201,11 @@
       <c r="H245" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="246" spans="1:8" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I245" s="5" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="246" spans="1:9" ht="91" x14ac:dyDescent="0.35">
       <c r="A246" s="3" t="s">
         <v>788</v>
       </c>
@@ -9438,8 +10230,11 @@
       <c r="H246" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="247" spans="1:8" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I246" s="5" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="247" spans="1:9" ht="78" x14ac:dyDescent="0.35">
       <c r="A247" s="3" t="s">
         <v>792</v>
       </c>
@@ -9464,8 +10259,11 @@
       <c r="H247" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="248" spans="1:8" ht="195.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I247" s="5" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="248" spans="1:9" ht="195" x14ac:dyDescent="0.35">
       <c r="A248" s="3" t="s">
         <v>795</v>
       </c>
@@ -9490,8 +10288,11 @@
       <c r="H248" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="249" spans="1:8" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I248" s="5" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="249" spans="1:9" ht="91" x14ac:dyDescent="0.35">
       <c r="A249" s="3" t="s">
         <v>798</v>
       </c>
@@ -9516,8 +10317,11 @@
       <c r="H249" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="250" spans="1:8" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I249" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="250" spans="1:9" ht="65" x14ac:dyDescent="0.35">
       <c r="A250" s="3" t="s">
         <v>802</v>
       </c>
@@ -9542,8 +10346,11 @@
       <c r="H250" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="251" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I250" s="5" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="251" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A251" s="3" t="s">
         <v>805</v>
       </c>
@@ -9568,8 +10375,11 @@
       <c r="H251" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="252" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I251" s="5" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="252" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A252" s="3" t="s">
         <v>808</v>
       </c>
@@ -9594,8 +10404,11 @@
       <c r="H252" s="4" t="s">
         <v>813</v>
       </c>
-    </row>
-    <row r="253" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I252" s="5" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="253" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A253" s="3" t="s">
         <v>814</v>
       </c>
@@ -9620,8 +10433,11 @@
       <c r="H253" s="4" t="s">
         <v>813</v>
       </c>
-    </row>
-    <row r="254" spans="1:8" ht="130.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I253" s="5" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="254" spans="1:9" ht="130" x14ac:dyDescent="0.35">
       <c r="A254" s="3" t="s">
         <v>817</v>
       </c>
@@ -9646,8 +10462,11 @@
       <c r="H254" s="4" t="s">
         <v>813</v>
       </c>
-    </row>
-    <row r="255" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I254" s="5" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="255" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A255" s="3" t="s">
         <v>820</v>
       </c>
@@ -9672,8 +10491,11 @@
       <c r="H255" s="4" t="s">
         <v>813</v>
       </c>
-    </row>
-    <row r="256" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I255" s="5" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="256" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A256" s="3" t="s">
         <v>823</v>
       </c>
@@ -9698,8 +10520,11 @@
       <c r="H256" s="4" t="s">
         <v>813</v>
       </c>
-    </row>
-    <row r="257" spans="1:8" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I256" s="5" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="257" spans="1:9" ht="78" x14ac:dyDescent="0.35">
       <c r="A257" s="3" t="s">
         <v>826</v>
       </c>
@@ -9724,8 +10549,11 @@
       <c r="H257" s="4" t="s">
         <v>813</v>
       </c>
-    </row>
-    <row r="258" spans="1:8" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I257" s="5" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="258" spans="1:9" ht="52" x14ac:dyDescent="0.35">
       <c r="A258" s="3" t="s">
         <v>829</v>
       </c>
@@ -9750,8 +10578,11 @@
       <c r="H258" s="4" t="s">
         <v>813</v>
       </c>
-    </row>
-    <row r="259" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I258" s="5" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="259" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A259" s="3" t="s">
         <v>832</v>
       </c>
@@ -9776,8 +10607,11 @@
       <c r="H259" s="4" t="s">
         <v>813</v>
       </c>
-    </row>
-    <row r="260" spans="1:8" ht="143.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I259" s="5" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="260" spans="1:9" ht="143" x14ac:dyDescent="0.35">
       <c r="A260" s="3" t="s">
         <v>836</v>
       </c>
@@ -9802,8 +10636,11 @@
       <c r="H260" s="4" t="s">
         <v>813</v>
       </c>
-    </row>
-    <row r="261" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I260" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="261" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A261" s="3" t="s">
         <v>839</v>
       </c>
@@ -9828,8 +10665,11 @@
       <c r="H261" s="4" t="s">
         <v>813</v>
       </c>
-    </row>
-    <row r="262" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I261" s="5" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="262" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A262" s="3" t="s">
         <v>842</v>
       </c>
@@ -9854,8 +10694,11 @@
       <c r="H262" s="4" t="s">
         <v>813</v>
       </c>
-    </row>
-    <row r="263" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I262" s="5" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="263" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A263" s="3" t="s">
         <v>845</v>
       </c>
@@ -9880,8 +10723,11 @@
       <c r="H263" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="264" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I263" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="264" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A264" s="3" t="s">
         <v>849</v>
       </c>
@@ -9906,8 +10752,11 @@
       <c r="H264" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="265" spans="1:8" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I264" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="265" spans="1:9" ht="39" x14ac:dyDescent="0.35">
       <c r="A265" s="3" t="s">
         <v>851</v>
       </c>
@@ -9931,6 +10780,9 @@
       </c>
       <c r="H265" s="4" t="s">
         <v>856</v>
+      </c>
+      <c r="I265" s="5" t="s">
+        <v>859</v>
       </c>
     </row>
   </sheetData>

</xml_diff>